<commit_message>
updated bulk upload file format and build script for frontend
</commit_message>
<xml_diff>
--- a/frontend/public/format.xlsx
+++ b/frontend/public/format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebApps\SmartmarkCRM\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE87AD25-E51F-48CD-932F-F866635ABCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FD61A7-1AEB-4D75-8598-84EC0D993EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="624" yWindow="624" windowWidth="21600" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>leadowneremail</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>source</t>
   </si>
@@ -385,22 +382,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="5" width="18.109375" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,96 +412,72 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6" s="2"/>
+      <c r="E6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="E22" s="2"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
domestic/international dropdown added, password change notification, warranty status + ivr ticket code + lead for added in lead form - update led and lead card, updated the bulk data upload sheet.
</commit_message>
<xml_diff>
--- a/frontend/public/format.xlsx
+++ b/frontend/public/format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebApps\SmartmarkCRM\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FD61A7-1AEB-4D75-8598-84EC0D993EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F377D56E-F916-4023-A7FA-460AE5D8C827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>source</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>territory</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>leadfor</t>
   </si>
 </sst>
 </file>
@@ -382,83 +391,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
-    <col min="3" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
       <c r="E6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added new user(Aniket S. Kulkarni) for chatbot/googleleads. Added the column header region and ivr ticket code in bulk upload sheet. Added region in the system.
</commit_message>
<xml_diff>
--- a/frontend/public/format.xlsx
+++ b/frontend/public/format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebApps\SmartmarkCRM\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F377D56E-F916-4023-A7FA-460AE5D8C827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF40D92E-B875-464D-8F6D-B72913B5A56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>source</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>leadfor</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>ivrticketcode</t>
   </si>
 </sst>
 </file>
@@ -391,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -403,12 +409,12 @@
     <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,67 +425,70 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
       <c r="E6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Changes - Bulkupload with all fields, combined firstname and lastname into the fullname, Updated UI(Version 2 Launched)
</commit_message>
<xml_diff>
--- a/frontend/public/format.xlsx
+++ b/frontend/public/format.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebApps\SmartmarkCRM\frontend\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Applications\SmartmarkCRM\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF40D92E-B875-464D-8F6D-B72913B5A56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3D2A48-8B7A-4D9D-B96D-71FEB9642787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1128" windowWidth="21600" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>source</t>
   </si>
   <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -58,6 +52,57 @@
   </si>
   <si>
     <t>ivrticketcode</t>
+  </si>
+  <si>
+    <t>leadowner</t>
+  </si>
+  <si>
+    <t>fullname</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>requirements</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>primarycategory</t>
+  </si>
+  <si>
+    <t>secondarycategory</t>
+  </si>
+  <si>
+    <t>whatsapp</t>
+  </si>
+  <si>
+    <t>designation</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>isfca</t>
+  </si>
+  <si>
+    <t>isivrticketopen</t>
+  </si>
+  <si>
+    <t>warrantystatus</t>
+  </si>
+  <si>
+    <t>domesticorexport</t>
+  </si>
+  <si>
+    <t>referredby</t>
+  </si>
+  <si>
+    <t>referrefto</t>
   </si>
 </sst>
 </file>
@@ -397,98 +442,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
       <c r="E6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.3">

</xml_diff>